<commit_message>
now admins can get access to the list of users
</commit_message>
<xml_diff>
--- a/users_list.xlsx
+++ b/users_list.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -453,23 +453,9 @@
         <v>Active</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Xusan</v>
-      </c>
-      <c r="B4">
-        <v>1753566525</v>
-      </c>
-      <c r="D4" t="str">
-        <v>request_contact</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Active</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>